<commit_message>
test on planned production function
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayman/Desktop/FYP_project/Vulcan/InitializationData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F7C1D6-14C0-3A40-93EE-27A4C62A3A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21592629-9E96-F440-A45C-36B4C0C93D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initialization_Parameters" sheetId="1" r:id="rId1"/>
@@ -1007,8 +1007,8 @@
   </sheetPr>
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1036,7 +1036,7 @@
         <v>93</v>
       </c>
       <c r="B3" s="2">
-        <v>0.02</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1282,7 +1282,7 @@
         <v>123</v>
       </c>
       <c r="B34" s="2">
-        <v>600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1833,8 +1833,8 @@
   </sheetPr>
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1862,7 +1862,7 @@
         <v>41</v>
       </c>
       <c r="B3" s="3">
-        <v>60</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixed initial nbr of workers in each firm
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayman/Desktop/FYP_project/Vulcan/InitializationData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090212B2-8D82-3B4E-A41A-C709565839EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EB0F72-8013-174F-8A5A-58AB28F597EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initialization_Parameters" sheetId="1" r:id="rId1"/>
@@ -1010,8 +1010,8 @@
   </sheetPr>
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1245,7 +1245,7 @@
         <v>118</v>
       </c>
       <c r="B29" s="2">
-        <v>950</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1253,7 +1253,7 @@
         <v>119</v>
       </c>
       <c r="B30" s="2">
-        <v>300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1261,7 +1261,7 @@
         <v>120</v>
       </c>
       <c r="B31" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1285,7 +1285,7 @@
         <v>123</v>
       </c>
       <c r="B34" s="2">
-        <v>600</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1379,7 +1379,8 @@
         <v>134</v>
       </c>
       <c r="B46" s="2">
-        <v>20</v>
+        <f>INT((Main_Loop_Parameters!B4-Main_Loop_Parameters!B7)/Main_Loop_Parameters!B7 )</f>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1387,7 +1388,7 @@
         <v>135</v>
       </c>
       <c r="B47" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1836,8 +1837,8 @@
   </sheetPr>
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1873,7 +1874,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="3">
-        <v>50</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1881,7 +1882,7 @@
         <v>43</v>
       </c>
       <c r="B5" s="3">
-        <v>12</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1889,7 +1890,7 @@
         <v>44</v>
       </c>
       <c r="B6" s="3">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1897,7 +1898,8 @@
         <v>45</v>
       </c>
       <c r="B7" s="3">
-        <v>16</v>
+        <f>B5+B6</f>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixed planned production order of magnitude
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayman/Desktop/FYP_project/Vulcan/InitializationData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D339865F-F705-7846-B415-72194B8D1613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A39FE0D-E976-1149-9D75-D7A36E442B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="186">
   <si>
     <t>sector_name</t>
   </si>
@@ -137,478 +137,463 @@
     <t>firm_cons_rand_price_change_upper_limit</t>
   </si>
   <si>
+    <t>Capital Firms</t>
+  </si>
+  <si>
+    <t>firm_cap_rand_sentiment_adoption</t>
+  </si>
+  <si>
+    <t>firm_cap_rand_desired_inventory_factor_change</t>
+  </si>
+  <si>
+    <t>firm_cap_rand_price_change_upper_limit</t>
+  </si>
+  <si>
+    <t>Simulation Parameters</t>
+  </si>
+  <si>
+    <t>Simulation Size and Length</t>
+  </si>
+  <si>
+    <t>n_loops</t>
+  </si>
+  <si>
+    <t>n_households</t>
+  </si>
+  <si>
+    <t>n_consumer_firms</t>
+  </si>
+  <si>
+    <t>n_capital_firms</t>
+  </si>
+  <si>
+    <t>n_firms</t>
+  </si>
+  <si>
+    <t>n_consumer_sectors</t>
+  </si>
+  <si>
+    <t>Dynamic Household Parameters</t>
+  </si>
+  <si>
+    <t>household_n_res_wage_decrease</t>
+  </si>
+  <si>
+    <t>household_targeted_savings_to_income_ratio</t>
+  </si>
+  <si>
+    <t>standard_employment_contract_length</t>
+  </si>
+  <si>
+    <t>firm_tax_rate</t>
+  </si>
+  <si>
+    <t>Consumer Firm Dynamic Parameters</t>
+  </si>
+  <si>
+    <t>firm_cons_inv_depr_rate</t>
+  </si>
+  <si>
+    <t>firm_cons_productivity</t>
+  </si>
+  <si>
+    <t>firm_cons_workers_per_machine</t>
+  </si>
+  <si>
+    <t>firm_cons_good_unit_cost</t>
+  </si>
+  <si>
+    <t>firm_cons_inv_reaction_factor</t>
+  </si>
+  <si>
+    <t>Capital Firm Dynamic Parameters</t>
+  </si>
+  <si>
+    <t>firm_cap_inv_depr_rate</t>
+  </si>
+  <si>
+    <t>firm_cap_productivity</t>
+  </si>
+  <si>
+    <t>firm_cap_workers_per_machine</t>
+  </si>
+  <si>
+    <t>firm_cap_good_unit_cost</t>
+  </si>
+  <si>
+    <t>firm_cap_machine_lifespan</t>
+  </si>
+  <si>
+    <t>firm_cap_inv_reaction_factor</t>
+  </si>
+  <si>
+    <t>Dynamic Bank Parameters</t>
+  </si>
+  <si>
+    <t>bank_inflation_reaction</t>
+  </si>
+  <si>
+    <t>bank_inflation_target</t>
+  </si>
+  <si>
+    <t>bank_inflation_target_monthly</t>
+  </si>
+  <si>
+    <t>bank_risk_premium</t>
+  </si>
+  <si>
+    <t>bank_short_term_loan_length</t>
+  </si>
+  <si>
+    <t>bank_long_term_loan_length</t>
+  </si>
+  <si>
+    <t>bank_leverage_ratio_lower_threshold</t>
+  </si>
+  <si>
+    <t>bank_leverage_ratio_upper_threshold</t>
+  </si>
+  <si>
+    <t>bank_max_interest_rate</t>
+  </si>
+  <si>
+    <t>bank_max_interest_rate_change</t>
+  </si>
+  <si>
+    <t>Bank Emission Penalty Parameters</t>
+  </si>
+  <si>
+    <t>bank_emission_penalty_max</t>
+  </si>
+  <si>
+    <t>bank_total_emission_penalty</t>
+  </si>
+  <si>
+    <t>bank_unit_emission_penalty</t>
+  </si>
+  <si>
+    <t>bank_unit_emission_lower_thr</t>
+  </si>
+  <si>
+    <t>bank_unit_emission_upper_thr</t>
+  </si>
+  <si>
+    <t>bank_total_emission_lower_thr</t>
+  </si>
+  <si>
+    <t>bank_total_emission_upper_thr</t>
+  </si>
+  <si>
+    <t>Emission Allowance Parameters</t>
+  </si>
+  <si>
+    <t>emission_total_allowance_change</t>
+  </si>
+  <si>
+    <t>emission_unit_price_change</t>
+  </si>
+  <si>
+    <t>Agent Initialization Parameters</t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>bank_init_interest_rate</t>
+  </si>
+  <si>
+    <t>household_init_c_f_mean</t>
+  </si>
+  <si>
+    <t>household_init_c_f_std</t>
+  </si>
+  <si>
+    <t>household_init_c_f_min</t>
+  </si>
+  <si>
+    <t>household_init_c_f_max</t>
+  </si>
+  <si>
+    <t>household_init_c_excess_mean</t>
+  </si>
+  <si>
+    <t>household_init_c_excess_std</t>
+  </si>
+  <si>
+    <t>household_init_c_excess_min</t>
+  </si>
+  <si>
+    <t>household_init_c_excess_max</t>
+  </si>
+  <si>
+    <t>household_init_s_optimist_mean</t>
+  </si>
+  <si>
+    <t>household_init_s_optimist_std</t>
+  </si>
+  <si>
+    <t>household_init_s_optimist_min</t>
+  </si>
+  <si>
+    <t>household_init_s_optimist_max</t>
+  </si>
+  <si>
+    <t>household_init_s_pessimist_mean</t>
+  </si>
+  <si>
+    <t>household_init_s_pessimist_std</t>
+  </si>
+  <si>
+    <t>household_init_s_pessimist_min</t>
+  </si>
+  <si>
+    <t>household_init_s_pessimist_max</t>
+  </si>
+  <si>
+    <t>household_init_wealth_mean</t>
+  </si>
+  <si>
+    <t>household_init_wealth_std</t>
+  </si>
+  <si>
+    <t>household_init_wealth_min</t>
+  </si>
+  <si>
+    <t>household_init_wealth_max</t>
+  </si>
+  <si>
+    <t>household_init_unemp_tolerance_mean</t>
+  </si>
+  <si>
+    <t>household_init_unemp_tolerance_std</t>
+  </si>
+  <si>
+    <t>household_init_unemp_tolerance_min</t>
+  </si>
+  <si>
+    <t>household_init_unemp_tolerance_max</t>
+  </si>
+  <si>
+    <t>household_init_res_wage_mean</t>
+  </si>
+  <si>
+    <t>household_init_res_wage_std</t>
+  </si>
+  <si>
+    <t>household_init_res_wage_min</t>
+  </si>
+  <si>
+    <t>household_init_res_wage_max</t>
+  </si>
+  <si>
+    <t>household_init_unemployment_benefit</t>
+  </si>
+  <si>
+    <t>household_init_minimum_wage</t>
+  </si>
+  <si>
+    <t>firm_cons_init_cash_mean</t>
+  </si>
+  <si>
+    <t>firm_cons_init_cash_std</t>
+  </si>
+  <si>
+    <t>firm_cons_init_cash_min</t>
+  </si>
+  <si>
+    <t>firm_cons_init_cash_max</t>
+  </si>
+  <si>
+    <t>firm_cons_init_dividend_ratio_optimist</t>
+  </si>
+  <si>
+    <t>firm_cons_init_dividend_ratio_pessimist</t>
+  </si>
+  <si>
+    <t>firm_cons_init_wage_offer_mean</t>
+  </si>
+  <si>
+    <t>firm_cons_init_wage_offer_std</t>
+  </si>
+  <si>
+    <t>firm_cons_init_wage_offer_min</t>
+  </si>
+  <si>
+    <t>firm_cons_init_wage_offer_max</t>
+  </si>
+  <si>
+    <t>firm_cons_init_worker_demand_mean</t>
+  </si>
+  <si>
+    <t>firm_cons_init_worker_demand_std</t>
+  </si>
+  <si>
+    <t>firm_cons_init_worker_demand_min</t>
+  </si>
+  <si>
+    <t>firm_cons_init_worker_demand_max</t>
+  </si>
+  <si>
+    <t>firm_cons_init_good_price_mean</t>
+  </si>
+  <si>
+    <t>firm_cons_init_good_price_std</t>
+  </si>
+  <si>
+    <t>firm_cons_init_good_price_min</t>
+  </si>
+  <si>
+    <t>firm_cons_init_good_price_max</t>
+  </si>
+  <si>
+    <t>firm_cons_init_inv_factor_mean</t>
+  </si>
+  <si>
+    <t>firm_cons_init_inv_factor_std</t>
+  </si>
+  <si>
+    <t>firm_cons_init_inv_factor_min</t>
+  </si>
+  <si>
+    <t>firm_cons_init_inv_factor_max</t>
+  </si>
+  <si>
+    <t>firm_cons_init_target_inv_factor_mean</t>
+  </si>
+  <si>
+    <t>firm_cons_init_target_inv_factor_std</t>
+  </si>
+  <si>
+    <t>firm_cons_init_target_inv_factor_min</t>
+  </si>
+  <si>
+    <t>firm_cons_init_target_inv_factor_max</t>
+  </si>
+  <si>
+    <t>firm_cons_init_production_current_ratio</t>
+  </si>
+  <si>
+    <t>firm_cons_init_quantity_sold_ratio</t>
+  </si>
+  <si>
+    <t>firm_cap_init_emissions_per_unit</t>
+  </si>
+  <si>
+    <t>firm_cap_init_cash_mean</t>
+  </si>
+  <si>
+    <t>firm_cap_init_cash_std</t>
+  </si>
+  <si>
+    <t>firm_cap_init_cash_min</t>
+  </si>
+  <si>
+    <t>firm_cap_init_cash_max</t>
+  </si>
+  <si>
+    <t>firm_cap_init_dividend_ratio_optimist</t>
+  </si>
+  <si>
+    <t>firm_cap_init_dividend_ratio_pessimist</t>
+  </si>
+  <si>
+    <t>firm_cap_init_wage_offer_mean</t>
+  </si>
+  <si>
+    <t>firm_cap_init_wage_offer_std</t>
+  </si>
+  <si>
+    <t>firm_cap_init_wage_offer_min</t>
+  </si>
+  <si>
+    <t>firm_cap_init_wage_offer_max</t>
+  </si>
+  <si>
+    <t>firm_cap_init_worker_demand_mean</t>
+  </si>
+  <si>
+    <t>firm_cap_init_worker_demand_std</t>
+  </si>
+  <si>
+    <t>firm_cap_init_worker_demand_min</t>
+  </si>
+  <si>
+    <t>firm_cap_init_worker_demand_max</t>
+  </si>
+  <si>
+    <t>firm_cap_init_good_price_mean</t>
+  </si>
+  <si>
+    <t>firm_cap_init_good_price_std</t>
+  </si>
+  <si>
+    <t>firm_cap_init_good_price_min</t>
+  </si>
+  <si>
+    <t>firm_cap_init_good_price_max</t>
+  </si>
+  <si>
+    <t>firm_cap_init_inv_factor_mean</t>
+  </si>
+  <si>
+    <t>firm_cap_init_inv_factor_std</t>
+  </si>
+  <si>
+    <t>firm_cap_init_inv_factor_min</t>
+  </si>
+  <si>
+    <t>firm_cap_init_inv_factor_max</t>
+  </si>
+  <si>
+    <t>firm_cap_init_target_inv_factor_mean</t>
+  </si>
+  <si>
+    <t>firm_cap_init_target_inv_factor_std</t>
+  </si>
+  <si>
+    <t>firm_cap_init_target_inv_factor_min</t>
+  </si>
+  <si>
+    <t>firm_cap_init_target_inv_factor_max</t>
+  </si>
+  <si>
+    <t>firm_cap_init_production_current_ratio</t>
+  </si>
+  <si>
+    <t>firm_cap_init_quantity_sold_ratio</t>
+  </si>
+  <si>
+    <t>CO2 Emission Sensitivities</t>
+  </si>
+  <si>
+    <t>emission_sensitivity_min</t>
+  </si>
+  <si>
+    <t>emission_sensitivity_max</t>
+  </si>
+  <si>
+    <t>emisssion_sensitivity_std</t>
+  </si>
+  <si>
+    <t>emission_sensitivity_threshold</t>
+  </si>
+  <si>
+    <t>Emission Allowances</t>
+  </si>
+  <si>
+    <t>emission_init_total_allowance</t>
+  </si>
+  <si>
+    <t>emission_init_unit_price</t>
+  </si>
+  <si>
+    <t>firm_cons_init_emissions_per_unit</t>
+  </si>
+  <si>
     <t>firm_cons_rand_wage_change</t>
   </si>
   <si>
-    <t>Capital Firms</t>
-  </si>
-  <si>
-    <t>firm_cap_rand_sentiment_adoption</t>
-  </si>
-  <si>
-    <t>firm_cap_rand_desired_inventory_factor_change</t>
-  </si>
-  <si>
-    <t>firm_cap_rand_price_change_upper_limit</t>
-  </si>
-  <si>
     <t>firm_cap_rand_wage_change</t>
-  </si>
-  <si>
-    <t>Simulation Parameters</t>
-  </si>
-  <si>
-    <t>Simulation Size and Length</t>
-  </si>
-  <si>
-    <t>n_loops</t>
-  </si>
-  <si>
-    <t>n_households</t>
-  </si>
-  <si>
-    <t>n_consumer_firms</t>
-  </si>
-  <si>
-    <t>n_capital_firms</t>
-  </si>
-  <si>
-    <t>n_firms</t>
-  </si>
-  <si>
-    <t>n_consumer_sectors</t>
-  </si>
-  <si>
-    <t>Dynamic Household Parameters</t>
-  </si>
-  <si>
-    <t>household_n_res_wage_decrease</t>
-  </si>
-  <si>
-    <t>household_targeted_savings_to_income_ratio</t>
-  </si>
-  <si>
-    <t>standard_employment_contract_length</t>
-  </si>
-  <si>
-    <t>firm_tax_rate</t>
-  </si>
-  <si>
-    <t>Consumer Firm Dynamic Parameters</t>
-  </si>
-  <si>
-    <t>firm_cons_inv_depr_rate</t>
-  </si>
-  <si>
-    <t>firm_cons_productivity</t>
-  </si>
-  <si>
-    <t>firm_cons_workers_per_machine</t>
-  </si>
-  <si>
-    <t>firm_cons_good_unit_cost</t>
-  </si>
-  <si>
-    <t>firm_cons_inv_reaction_factor</t>
-  </si>
-  <si>
-    <t>firm_cons_fixed_wage_change</t>
-  </si>
-  <si>
-    <t>firm_cons_fixed_price_change</t>
-  </si>
-  <si>
-    <t>Capital Firm Dynamic Parameters</t>
-  </si>
-  <si>
-    <t>firm_cap_inv_depr_rate</t>
-  </si>
-  <si>
-    <t>firm_cap_productivity</t>
-  </si>
-  <si>
-    <t>firm_cap_workers_per_machine</t>
-  </si>
-  <si>
-    <t>firm_cap_good_unit_cost</t>
-  </si>
-  <si>
-    <t>firm_cap_machine_lifespan</t>
-  </si>
-  <si>
-    <t>firm_cap_inv_reaction_factor</t>
-  </si>
-  <si>
-    <t>firm_cap_fixed_wage_change</t>
-  </si>
-  <si>
-    <t>firm_cap_fixed_price_change</t>
-  </si>
-  <si>
-    <t>Dynamic Bank Parameters</t>
-  </si>
-  <si>
-    <t>bank_inflation_reaction</t>
-  </si>
-  <si>
-    <t>bank_inflation_target</t>
-  </si>
-  <si>
-    <t>bank_inflation_target_monthly</t>
-  </si>
-  <si>
-    <t>bank_risk_premium</t>
-  </si>
-  <si>
-    <t>bank_short_term_loan_length</t>
-  </si>
-  <si>
-    <t>bank_long_term_loan_length</t>
-  </si>
-  <si>
-    <t>bank_leverage_ratio_lower_threshold</t>
-  </si>
-  <si>
-    <t>bank_leverage_ratio_upper_threshold</t>
-  </si>
-  <si>
-    <t>bank_max_interest_rate</t>
-  </si>
-  <si>
-    <t>bank_max_interest_rate_change</t>
-  </si>
-  <si>
-    <t>Bank Emission Penalty Parameters</t>
-  </si>
-  <si>
-    <t>bank_emission_penalty_max</t>
-  </si>
-  <si>
-    <t>bank_total_emission_penalty</t>
-  </si>
-  <si>
-    <t>bank_unit_emission_penalty</t>
-  </si>
-  <si>
-    <t>bank_unit_emission_lower_thr</t>
-  </si>
-  <si>
-    <t>bank_unit_emission_upper_thr</t>
-  </si>
-  <si>
-    <t>bank_total_emission_lower_thr</t>
-  </si>
-  <si>
-    <t>bank_total_emission_upper_thr</t>
-  </si>
-  <si>
-    <t>Emission Allowance Parameters</t>
-  </si>
-  <si>
-    <t>emission_total_allowance_change</t>
-  </si>
-  <si>
-    <t>emission_unit_price_change</t>
-  </si>
-  <si>
-    <t>Agent Initialization Parameters</t>
-  </si>
-  <si>
-    <t>Bank</t>
-  </si>
-  <si>
-    <t>bank_init_interest_rate</t>
-  </si>
-  <si>
-    <t>household_init_c_f_mean</t>
-  </si>
-  <si>
-    <t>household_init_c_f_std</t>
-  </si>
-  <si>
-    <t>household_init_c_f_min</t>
-  </si>
-  <si>
-    <t>household_init_c_f_max</t>
-  </si>
-  <si>
-    <t>household_init_c_excess_mean</t>
-  </si>
-  <si>
-    <t>household_init_c_excess_std</t>
-  </si>
-  <si>
-    <t>household_init_c_excess_min</t>
-  </si>
-  <si>
-    <t>household_init_c_excess_max</t>
-  </si>
-  <si>
-    <t>household_init_s_optimist_mean</t>
-  </si>
-  <si>
-    <t>household_init_s_optimist_std</t>
-  </si>
-  <si>
-    <t>household_init_s_optimist_min</t>
-  </si>
-  <si>
-    <t>household_init_s_optimist_max</t>
-  </si>
-  <si>
-    <t>household_init_s_pessimist_mean</t>
-  </si>
-  <si>
-    <t>household_init_s_pessimist_std</t>
-  </si>
-  <si>
-    <t>household_init_s_pessimist_min</t>
-  </si>
-  <si>
-    <t>household_init_s_pessimist_max</t>
-  </si>
-  <si>
-    <t>household_init_wealth_mean</t>
-  </si>
-  <si>
-    <t>household_init_wealth_std</t>
-  </si>
-  <si>
-    <t>household_init_wealth_min</t>
-  </si>
-  <si>
-    <t>household_init_wealth_max</t>
-  </si>
-  <si>
-    <t>household_init_unemp_tolerance_mean</t>
-  </si>
-  <si>
-    <t>household_init_unemp_tolerance_std</t>
-  </si>
-  <si>
-    <t>household_init_unemp_tolerance_min</t>
-  </si>
-  <si>
-    <t>household_init_unemp_tolerance_max</t>
-  </si>
-  <si>
-    <t>household_init_res_wage_mean</t>
-  </si>
-  <si>
-    <t>household_init_res_wage_std</t>
-  </si>
-  <si>
-    <t>household_init_res_wage_min</t>
-  </si>
-  <si>
-    <t>household_init_res_wage_max</t>
-  </si>
-  <si>
-    <t>household_init_unemployment_benefit</t>
-  </si>
-  <si>
-    <t>household_init_minimum_wage</t>
-  </si>
-  <si>
-    <t>firm_cons_init_cash_mean</t>
-  </si>
-  <si>
-    <t>firm_cons_init_cash_std</t>
-  </si>
-  <si>
-    <t>firm_cons_init_cash_min</t>
-  </si>
-  <si>
-    <t>firm_cons_init_cash_max</t>
-  </si>
-  <si>
-    <t>firm_cons_init_dividend_ratio_optimist</t>
-  </si>
-  <si>
-    <t>firm_cons_init_dividend_ratio_pessimist</t>
-  </si>
-  <si>
-    <t>firm_cons_init_wage_offer_mean</t>
-  </si>
-  <si>
-    <t>firm_cons_init_wage_offer_std</t>
-  </si>
-  <si>
-    <t>firm_cons_init_wage_offer_min</t>
-  </si>
-  <si>
-    <t>firm_cons_init_wage_offer_max</t>
-  </si>
-  <si>
-    <t>firm_cons_init_worker_demand_mean</t>
-  </si>
-  <si>
-    <t>firm_cons_init_worker_demand_std</t>
-  </si>
-  <si>
-    <t>firm_cons_init_worker_demand_min</t>
-  </si>
-  <si>
-    <t>firm_cons_init_worker_demand_max</t>
-  </si>
-  <si>
-    <t>firm_cons_init_good_price_mean</t>
-  </si>
-  <si>
-    <t>firm_cons_init_good_price_std</t>
-  </si>
-  <si>
-    <t>firm_cons_init_good_price_min</t>
-  </si>
-  <si>
-    <t>firm_cons_init_good_price_max</t>
-  </si>
-  <si>
-    <t>firm_cons_init_inv_factor_mean</t>
-  </si>
-  <si>
-    <t>firm_cons_init_inv_factor_std</t>
-  </si>
-  <si>
-    <t>firm_cons_init_inv_factor_min</t>
-  </si>
-  <si>
-    <t>firm_cons_init_inv_factor_max</t>
-  </si>
-  <si>
-    <t>firm_cons_init_target_inv_factor_mean</t>
-  </si>
-  <si>
-    <t>firm_cons_init_target_inv_factor_std</t>
-  </si>
-  <si>
-    <t>firm_cons_init_target_inv_factor_min</t>
-  </si>
-  <si>
-    <t>firm_cons_init_target_inv_factor_max</t>
-  </si>
-  <si>
-    <t>firm_cons_init_production_current_ratio</t>
-  </si>
-  <si>
-    <t>firm_cons_init_quantity_sold_ratio</t>
-  </si>
-  <si>
-    <t>firm_cons_init_emissions_per_unit</t>
-  </si>
-  <si>
-    <t>firm_cap_init_cash_mean</t>
-  </si>
-  <si>
-    <t>firm_cap_init_cash_std</t>
-  </si>
-  <si>
-    <t>firm_cap_init_cash_min</t>
-  </si>
-  <si>
-    <t>firm_cap_init_cash_max</t>
-  </si>
-  <si>
-    <t>firm_cap_init_dividend_ratio_optimist</t>
-  </si>
-  <si>
-    <t>firm_cap_init_dividend_ratio_pessimist</t>
-  </si>
-  <si>
-    <t>firm_cap_init_wage_offer_mean</t>
-  </si>
-  <si>
-    <t>firm_cap_init_wage_offer_std</t>
-  </si>
-  <si>
-    <t>firm_cap_init_wage_offer_min</t>
-  </si>
-  <si>
-    <t>firm_cap_init_wage_offer_max</t>
-  </si>
-  <si>
-    <t>firm_cap_init_worker_demand_mean</t>
-  </si>
-  <si>
-    <t>firm_cap_init_worker_demand_std</t>
-  </si>
-  <si>
-    <t>firm_cap_init_worker_demand_min</t>
-  </si>
-  <si>
-    <t>firm_cap_init_worker_demand_max</t>
-  </si>
-  <si>
-    <t>firm_cap_init_good_price_mean</t>
-  </si>
-  <si>
-    <t>firm_cap_init_good_price_std</t>
-  </si>
-  <si>
-    <t>firm_cap_init_good_price_min</t>
-  </si>
-  <si>
-    <t>firm_cap_init_good_price_max</t>
-  </si>
-  <si>
-    <t>firm_cap_init_inv_factor_mean</t>
-  </si>
-  <si>
-    <t>firm_cap_init_inv_factor_std</t>
-  </si>
-  <si>
-    <t>firm_cap_init_inv_factor_min</t>
-  </si>
-  <si>
-    <t>firm_cap_init_inv_factor_max</t>
-  </si>
-  <si>
-    <t>firm_cap_init_target_inv_factor_mean</t>
-  </si>
-  <si>
-    <t>firm_cap_init_target_inv_factor_std</t>
-  </si>
-  <si>
-    <t>firm_cap_init_target_inv_factor_min</t>
-  </si>
-  <si>
-    <t>firm_cap_init_target_inv_factor_max</t>
-  </si>
-  <si>
-    <t>firm_cap_init_production_current_ratio</t>
-  </si>
-  <si>
-    <t>firm_cap_init_quantity_sold_ratio</t>
-  </si>
-  <si>
-    <t>firm_cap_init_emissions_per_unit</t>
-  </si>
-  <si>
-    <t>CO2 Emission Sensitivities</t>
-  </si>
-  <si>
-    <t>emission_sensitivity_min</t>
-  </si>
-  <si>
-    <t>emission_sensitivity_max</t>
-  </si>
-  <si>
-    <t>emisssion_sensitivity_std</t>
-  </si>
-  <si>
-    <t>emission_sensitivity_threshold</t>
-  </si>
-  <si>
-    <t>Emission Allowances</t>
-  </si>
-  <si>
-    <t>emission_init_total_allowance</t>
-  </si>
-  <si>
-    <t>emission_init_unit_price</t>
-  </si>
-  <si>
-    <t>0.05</t>
   </si>
 </sst>
 </file>
@@ -641,18 +626,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -674,7 +653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -697,7 +676,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -706,10 +685,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1015,10 +1002,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1029,24 +1016,24 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>190</v>
+        <v>87</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.02</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1057,7 +1044,7 @@
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B5" s="2">
         <v>0.5</v>
@@ -1065,7 +1052,7 @@
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B6" s="2">
         <v>0.1</v>
@@ -1073,7 +1060,7 @@
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B7" s="2">
         <v>0.1</v>
@@ -1081,7 +1068,7 @@
     </row>
     <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B8" s="2">
         <v>0.9</v>
@@ -1089,7 +1076,7 @@
     </row>
     <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B9" s="2">
         <v>0.3</v>
@@ -1097,7 +1084,7 @@
     </row>
     <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B10" s="2">
         <v>0.05</v>
@@ -1105,7 +1092,7 @@
     </row>
     <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B11" s="2">
         <v>0</v>
@@ -1113,7 +1100,7 @@
     </row>
     <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B12" s="2">
         <v>0.7</v>
@@ -1121,7 +1108,7 @@
     </row>
     <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B13" s="2">
         <v>0.2</v>
@@ -1129,7 +1116,7 @@
     </row>
     <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B14" s="2">
         <v>0.05</v>
@@ -1137,7 +1124,7 @@
     </row>
     <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B15" s="2">
         <v>0</v>
@@ -1145,7 +1132,7 @@
     </row>
     <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B16" s="2">
         <v>0.5</v>
@@ -1153,7 +1140,7 @@
     </row>
     <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B17" s="2">
         <v>0.3</v>
@@ -1161,7 +1148,7 @@
     </row>
     <row r="18" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B18" s="2">
         <v>0.05</v>
@@ -1169,7 +1156,7 @@
     </row>
     <row r="19" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B19" s="2">
         <v>0.1</v>
@@ -1177,7 +1164,7 @@
     </row>
     <row r="20" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B20" s="2">
         <v>0.6</v>
@@ -1185,7 +1172,7 @@
     </row>
     <row r="21" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B21" s="2">
         <v>1000</v>
@@ -1193,7 +1180,7 @@
     </row>
     <row r="22" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B22" s="2">
         <v>300</v>
@@ -1201,7 +1188,7 @@
     </row>
     <row r="23" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B23" s="2">
         <v>0</v>
@@ -1209,7 +1196,7 @@
     </row>
     <row r="24" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B24" s="2">
         <v>2000</v>
@@ -1217,7 +1204,7 @@
     </row>
     <row r="25" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B25" s="2">
         <v>4</v>
@@ -1225,7 +1212,7 @@
     </row>
     <row r="26" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B26" s="2">
         <v>2</v>
@@ -1233,7 +1220,7 @@
     </row>
     <row r="27" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B27" s="2">
         <v>0</v>
@@ -1241,7 +1228,7 @@
     </row>
     <row r="28" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B28" s="2">
         <v>100</v>
@@ -1249,31 +1236,31 @@
     </row>
     <row r="29" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B29" s="2">
-        <v>0</v>
+        <v>950</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B30" s="2">
-        <v>0</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B31" s="2">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B32" s="2">
         <v>999999</v>
@@ -1281,7 +1268,7 @@
     </row>
     <row r="33" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B33" s="2">
         <v>500</v>
@@ -1289,10 +1276,10 @@
     </row>
     <row r="34" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B34" s="2">
-        <v>1</v>
+        <v>600</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1303,23 +1290,23 @@
     </row>
     <row r="36" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B36" s="2">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B37" s="2">
-        <v>250</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B38" s="2">
         <v>1</v>
@@ -1327,7 +1314,7 @@
     </row>
     <row r="39" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B39" s="2">
         <v>999999999</v>
@@ -1335,7 +1322,7 @@
     </row>
     <row r="40" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B40" s="2">
         <v>0.01</v>
@@ -1343,7 +1330,7 @@
     </row>
     <row r="41" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B41" s="2">
         <v>5.0000000000000001E-3</v>
@@ -1351,7 +1338,7 @@
     </row>
     <row r="42" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B42" s="2">
         <v>1000</v>
@@ -1359,7 +1346,7 @@
     </row>
     <row r="43" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B43" s="2">
         <v>300</v>
@@ -1367,7 +1354,7 @@
     </row>
     <row r="44" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B44" s="2">
         <v>100</v>
@@ -1375,7 +1362,7 @@
     </row>
     <row r="45" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B45" s="2">
         <v>999999</v>
@@ -1383,153 +1370,151 @@
     </row>
     <row r="46" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B46" s="2">
-        <f>INT((Main_Loop_Parameters!B4-Main_Loop_Parameters!B7)/Main_Loop_Parameters!B7 )</f>
-        <v>61</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B47" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B48" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B49" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B50" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>139</v>
-      </c>
-      <c r="B51" s="11">
+        <v>133</v>
+      </c>
+      <c r="B51" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B52" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B53" s="2">
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B54" s="2">
-        <v>1</v>
-      </c>
-      <c r="C54" s="12"/>
-    </row>
-    <row r="55" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B55" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B56" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B57" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B58" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B59" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B60" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B61" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B62" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B63" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>152</v>
+        <v>183</v>
       </c>
       <c r="B64" s="2">
         <v>10</v>
@@ -1537,29 +1522,29 @@
     </row>
     <row r="65" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B65" s="3"/>
     </row>
     <row r="66" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B66" s="2">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B67" s="2">
-        <v>250</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B68" s="2">
         <v>1</v>
@@ -1567,7 +1552,7 @@
     </row>
     <row r="69" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B69" s="2">
         <v>999999999</v>
@@ -1575,7 +1560,7 @@
     </row>
     <row r="70" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B70" s="2">
         <v>0.04</v>
@@ -1583,7 +1568,7 @@
     </row>
     <row r="71" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B71" s="2">
         <v>0.01</v>
@@ -1591,7 +1576,7 @@
     </row>
     <row r="72" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B72" s="2">
         <v>1000</v>
@@ -1599,7 +1584,7 @@
     </row>
     <row r="73" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B73" s="2">
         <v>300</v>
@@ -1607,7 +1592,7 @@
     </row>
     <row r="74" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B74" s="2">
         <v>100</v>
@@ -1615,7 +1600,7 @@
     </row>
     <row r="75" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B75" s="2">
         <v>999999</v>
@@ -1623,23 +1608,23 @@
     </row>
     <row r="76" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B76" s="2">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B77" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B78" s="2">
         <v>1</v>
@@ -1647,7 +1632,7 @@
     </row>
     <row r="79" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B79" s="2">
         <v>100</v>
@@ -1655,7 +1640,7 @@
     </row>
     <row r="80" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B80" s="2">
         <v>2000</v>
@@ -1663,7 +1648,7 @@
     </row>
     <row r="81" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B81" s="2">
         <v>200</v>
@@ -1671,7 +1656,7 @@
     </row>
     <row r="82" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B82" s="2">
         <v>100</v>
@@ -1679,7 +1664,7 @@
     </row>
     <row r="83" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B83" s="2">
         <v>9999</v>
@@ -1687,7 +1672,7 @@
     </row>
     <row r="84" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B84" s="2">
         <v>1</v>
@@ -1695,7 +1680,7 @@
     </row>
     <row r="85" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B85" s="2">
         <v>0.25</v>
@@ -1703,7 +1688,7 @@
     </row>
     <row r="86" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B86" s="2">
         <v>0.1</v>
@@ -1711,7 +1696,7 @@
     </row>
     <row r="87" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B87" s="2">
         <v>2</v>
@@ -1719,7 +1704,7 @@
     </row>
     <row r="88" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B88" s="2">
         <v>1.5</v>
@@ -1727,7 +1712,7 @@
     </row>
     <row r="89" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B89" s="2">
         <v>0.25</v>
@@ -1735,7 +1720,7 @@
     </row>
     <row r="90" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B90" s="2">
         <v>0.1</v>
@@ -1743,7 +1728,7 @@
     </row>
     <row r="91" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B91" s="2">
         <v>4</v>
@@ -1751,7 +1736,7 @@
     </row>
     <row r="92" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B92" s="2">
         <v>0.4</v>
@@ -1759,7 +1744,7 @@
     </row>
     <row r="93" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B93" s="2">
         <v>0.25</v>
@@ -1767,7 +1752,7 @@
     </row>
     <row r="94" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
       <c r="B94" s="2">
         <v>100</v>
@@ -1775,13 +1760,13 @@
     </row>
     <row r="95" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B95" s="3"/>
     </row>
     <row r="96" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B96" s="2">
         <v>0</v>
@@ -1789,7 +1774,7 @@
     </row>
     <row r="97" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B97" s="2">
         <v>0.5</v>
@@ -1797,7 +1782,7 @@
     </row>
     <row r="98" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B98" s="2">
         <v>0.1</v>
@@ -1805,7 +1790,7 @@
     </row>
     <row r="99" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B99" s="2">
         <v>0.05</v>
@@ -1813,13 +1798,13 @@
     </row>
     <row r="100" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B100" s="3"/>
     </row>
     <row r="101" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B101" s="3">
         <v>1000000</v>
@@ -1827,7 +1812,7 @@
     </row>
     <row r="102" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B102" s="3">
         <v>0.5</v>
@@ -1843,10 +1828,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1857,37 +1842,37 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" s="3">
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4" s="3">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5" s="3">
         <v>12</v>
@@ -1895,7 +1880,7 @@
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6" s="3">
         <v>4</v>
@@ -1903,7 +1888,7 @@
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7" s="3">
         <f>B5+B6</f>
@@ -1912,7 +1897,7 @@
     </row>
     <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8" s="3">
         <v>12</v>
@@ -1920,13 +1905,13 @@
     </row>
     <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" s="3">
         <v>0.05</v>
@@ -1934,7 +1919,7 @@
     </row>
     <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
@@ -1942,7 +1927,7 @@
     </row>
     <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B12" s="3">
         <v>12</v>
@@ -1950,7 +1935,7 @@
     </row>
     <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" s="3">
         <v>0.2</v>
@@ -1958,13 +1943,13 @@
     </row>
     <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B15" s="3">
         <v>0.01</v>
@@ -1972,15 +1957,15 @@
     </row>
     <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B16" s="3">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
@@ -1988,7 +1973,7 @@
     </row>
     <row r="18" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
@@ -1996,171 +1981,169 @@
     </row>
     <row r="19" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B19" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="3">
-        <v>0.05</v>
-      </c>
+      <c r="A20" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B21" s="3">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="3"/>
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="23" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B23" s="3">
-        <v>0.01</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B24" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B25" s="3">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B26" s="3">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>65</v>
-      </c>
-      <c r="B27" s="3">
-        <v>100</v>
-      </c>
+      <c r="A27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="3"/>
     </row>
     <row r="28" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B28" s="3">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B29" s="3">
-        <v>0.05</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B30" s="3">
-        <v>0.05</v>
+        <v>1.004</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" s="3"/>
+      <c r="A31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="32" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B32" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B33" s="3">
-        <v>1.1000000000000001</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B34" s="3">
-        <v>1.008</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B35" s="3">
-        <v>0.05</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B36" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B37" s="3">
-        <v>24</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>76</v>
-      </c>
-      <c r="B38" s="3">
-        <v>10</v>
-      </c>
+      <c r="A38" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="3"/>
     </row>
     <row r="39" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B39" s="3">
-        <v>40</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B40" s="3">
         <v>1</v>
@@ -2168,93 +2151,63 @@
     </row>
     <row r="41" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B41" s="3">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" s="3"/>
+      <c r="A42" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B43" s="3">
-        <v>0.02</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B44" s="3">
-        <v>1</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B45" s="3">
-        <v>0</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>84</v>
-      </c>
-      <c r="B46" s="3">
-        <v>1</v>
-      </c>
+      <c r="A46" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="3"/>
     </row>
     <row r="47" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B47" s="3">
-        <v>10</v>
+        <v>-1E-3</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B48" s="3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>87</v>
-      </c>
-      <c r="B49" s="3">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B50" s="3"/>
-    </row>
-    <row r="51" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>89</v>
-      </c>
-      <c r="B51" s="3">
-        <v>-1E-3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>90</v>
-      </c>
-      <c r="B52" s="3">
         <v>1E-3</v>
       </c>
     </row>
@@ -2270,14 +2223,14 @@
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2299,7 +2252,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="9">
-        <v>5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2323,7 +2276,7 @@
         <v>27</v>
       </c>
       <c r="B6" s="9">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2361,20 +2314,20 @@
         <v>32</v>
       </c>
       <c r="B11" s="9">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="9">
+        <v>184</v>
+      </c>
+      <c r="B12" s="3">
         <v>0.25</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="9"/>
     </row>
@@ -2388,7 +2341,7 @@
     </row>
     <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="9">
         <v>0.1</v>
@@ -2396,7 +2349,7 @@
     </row>
     <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="9">
         <v>0.1</v>
@@ -2404,17 +2357,17 @@
     </row>
     <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="9">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="9">
+        <v>185</v>
+      </c>
+      <c r="B18" s="3">
         <v>0.25</v>
       </c>
     </row>
@@ -2428,10 +2381,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E13"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2484,10 +2437,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <v>8.3333333333333329E-2</v>
+        <v>0.08</v>
       </c>
       <c r="D2" s="3">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="E2" s="1">
         <v>100</v>
@@ -2496,7 +2449,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="1">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2">
         <v>0.1</v>
@@ -2513,19 +2466,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="2">
-        <v>8.3333333333333329E-2</v>
+        <v>0.08</v>
       </c>
       <c r="D3" s="3">
         <v>0.01</v>
       </c>
       <c r="E3" s="1">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
       </c>
       <c r="G3" s="1">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="H3" s="2">
         <v>0.1</v>
@@ -2542,22 +2495,22 @@
         <v>2</v>
       </c>
       <c r="C4" s="2">
-        <v>8.3333333333333329E-2</v>
+        <v>0.08</v>
       </c>
       <c r="D4" s="3">
         <v>0.01</v>
       </c>
       <c r="E4" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
       </c>
       <c r="G4" s="1">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H4" s="2">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I4" s="1">
         <v>48000</v>
@@ -2571,22 +2524,22 @@
         <v>3</v>
       </c>
       <c r="C5" s="2">
-        <v>8.3333333333333329E-2</v>
+        <v>0.08</v>
       </c>
       <c r="D5" s="3">
         <v>0.01</v>
       </c>
       <c r="E5" s="1">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
       <c r="G5" s="1">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="H5" s="2">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="I5" s="1">
         <v>303000</v>
@@ -2600,22 +2553,22 @@
         <v>4</v>
       </c>
       <c r="C6" s="2">
-        <v>8.3333333333333329E-2</v>
+        <v>0.08</v>
       </c>
       <c r="D6" s="3">
         <v>0.01</v>
       </c>
       <c r="E6" s="1">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
       </c>
       <c r="G6" s="1">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="H6" s="2">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I6" s="1">
         <v>56000</v>
@@ -2629,22 +2582,22 @@
         <v>5</v>
       </c>
       <c r="C7" s="2">
-        <v>8.3333333333333329E-2</v>
+        <v>0.08</v>
       </c>
       <c r="D7" s="3">
         <v>0.01</v>
       </c>
       <c r="E7" s="1">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
       </c>
       <c r="G7" s="1">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="H7" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I7" s="1">
         <v>18000</v>
@@ -2658,13 +2611,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="2">
-        <v>8.3333333333333329E-2</v>
+        <v>0.08</v>
       </c>
       <c r="D8" s="3">
         <v>0.01</v>
       </c>
       <c r="E8" s="1">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
@@ -2673,7 +2626,7 @@
         <v>50</v>
       </c>
       <c r="H8" s="2">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I8" s="1">
         <v>111000</v>
@@ -2687,22 +2640,22 @@
         <v>7</v>
       </c>
       <c r="C9" s="2">
-        <v>8.3333333333333329E-2</v>
+        <v>0.08</v>
       </c>
       <c r="D9" s="3">
         <v>0.01</v>
       </c>
       <c r="E9" s="1">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
       <c r="G9" s="1">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="H9" s="2">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="I9" s="1">
         <v>19000</v>
@@ -2716,19 +2669,19 @@
         <v>8</v>
       </c>
       <c r="C10" s="2">
-        <v>8.3333333333333329E-2</v>
+        <v>0.08</v>
       </c>
       <c r="D10" s="3">
         <v>0.01</v>
       </c>
       <c r="E10" s="1">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
       </c>
       <c r="G10" s="1">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="H10" s="2">
         <v>0.1</v>
@@ -2745,22 +2698,22 @@
         <v>9</v>
       </c>
       <c r="C11" s="2">
-        <v>8.3333333333333329E-2</v>
+        <v>0.08</v>
       </c>
       <c r="D11" s="3">
         <v>0.01</v>
       </c>
       <c r="E11" s="1">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
       </c>
       <c r="G11" s="1">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="H11" s="2">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I11" s="1">
         <v>23000</v>
@@ -2774,19 +2727,19 @@
         <v>10</v>
       </c>
       <c r="C12" s="2">
-        <v>8.3333333333333329E-2</v>
+        <v>0.08</v>
       </c>
       <c r="D12" s="3">
         <v>0.01</v>
       </c>
       <c r="E12" s="1">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
       </c>
       <c r="G12" s="1">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="H12" s="2">
         <v>0.1</v>
@@ -2803,85 +2756,25 @@
         <v>11</v>
       </c>
       <c r="C13" s="2">
-        <v>8.3333333333333329E-2</v>
+        <v>0.08</v>
       </c>
       <c r="D13" s="3">
         <v>0.01</v>
       </c>
       <c r="E13" s="1">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
       </c>
       <c r="G13" s="1">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="H13" s="2">
         <v>0.1</v>
       </c>
       <c r="I13" s="1">
         <v>67000</v>
-      </c>
-    </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="2">
-        <v>9.6000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="2">
-        <v>3.5000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="2">
-        <v>4.8000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="2">
-        <v>0.30299999999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="2">
-        <v>5.6000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="2">
-        <v>1.7999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="2">
-        <v>0.111</v>
-      </c>
-    </row>
-    <row r="30" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F30" s="2">
-        <v>1.9E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F31" s="2">
-        <v>0.112</v>
-      </c>
-    </row>
-    <row r="32" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F32" s="2">
-        <v>2.3E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F33" s="2">
-        <v>0.112</v>
-      </c>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F34" s="2">
-        <v>6.7000000000000004E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing to check production values
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayman/Desktop/FYP_project/Vulcan/InitializationData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A39FE0D-E976-1149-9D75-D7A36E442B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D87F3ED-6411-1740-ADDF-3830811DF9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initialization_Parameters" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="188">
   <si>
     <t>sector_name</t>
   </si>
@@ -594,6 +594,12 @@
   </si>
   <si>
     <t>firm_cap_rand_wage_change</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>0.02</t>
   </si>
 </sst>
 </file>
@@ -626,12 +632,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -653,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -695,6 +707,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="4" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1004,8 +1020,8 @@
   </sheetPr>
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="115" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1032,8 +1048,8 @@
       <c r="A3" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.02</v>
+      <c r="B3" s="2" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1055,7 +1071,7 @@
         <v>89</v>
       </c>
       <c r="B6" s="2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1087,7 +1103,7 @@
         <v>93</v>
       </c>
       <c r="B10" s="2">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1119,7 +1135,7 @@
         <v>97</v>
       </c>
       <c r="B14" s="2">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1151,7 +1167,7 @@
         <v>101</v>
       </c>
       <c r="B18" s="2">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1171,11 +1187,11 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="B21" s="2">
-        <v>1000</v>
+      <c r="B21" s="16">
+        <v>500</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1183,7 +1199,7 @@
         <v>105</v>
       </c>
       <c r="B22" s="2">
-        <v>300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1215,7 +1231,7 @@
         <v>109</v>
       </c>
       <c r="B26" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1239,7 +1255,7 @@
         <v>112</v>
       </c>
       <c r="B29" s="2">
-        <v>950</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1247,7 +1263,7 @@
         <v>113</v>
       </c>
       <c r="B30" s="2">
-        <v>300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1255,7 +1271,7 @@
         <v>114</v>
       </c>
       <c r="B31" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1279,7 +1295,7 @@
         <v>117</v>
       </c>
       <c r="B34" s="2">
-        <v>600</v>
+        <v>500</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1289,10 +1305,10 @@
       <c r="B35" s="3"/>
     </row>
     <row r="36" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="A36" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="16">
         <v>10000</v>
       </c>
     </row>
@@ -1301,7 +1317,7 @@
         <v>119</v>
       </c>
       <c r="B37" s="2">
-        <v>2500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1341,7 +1357,7 @@
         <v>124</v>
       </c>
       <c r="B42" s="2">
-        <v>1000</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1349,7 +1365,7 @@
         <v>125</v>
       </c>
       <c r="B43" s="2">
-        <v>300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1373,7 +1389,8 @@
         <v>128</v>
       </c>
       <c r="B46" s="2">
-        <v>20</v>
+        <f>INT(Main_Loop_Parameters!B4/Main_Loop_Parameters!B7)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1381,7 +1398,7 @@
         <v>129</v>
       </c>
       <c r="B47" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1397,7 +1414,7 @@
         <v>131</v>
       </c>
       <c r="B49" s="2">
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1405,7 +1422,7 @@
         <v>132</v>
       </c>
       <c r="B50" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1413,7 +1430,7 @@
         <v>133</v>
       </c>
       <c r="B51" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1429,7 +1446,7 @@
         <v>135</v>
       </c>
       <c r="B53" s="2">
-        <v>99</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1437,7 +1454,7 @@
         <v>136</v>
       </c>
       <c r="B54" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1445,7 +1462,7 @@
         <v>137</v>
       </c>
       <c r="B55" s="2">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1469,7 +1486,7 @@
         <v>140</v>
       </c>
       <c r="B58" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1477,7 +1494,7 @@
         <v>141</v>
       </c>
       <c r="B59" s="2">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1509,7 +1526,7 @@
         <v>145</v>
       </c>
       <c r="B63" s="2">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1527,10 +1544,10 @@
       <c r="B65" s="3"/>
     </row>
     <row r="66" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="A66" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66" s="16">
         <v>10000</v>
       </c>
     </row>
@@ -1539,7 +1556,7 @@
         <v>148</v>
       </c>
       <c r="B67" s="2">
-        <v>2500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1579,7 +1596,7 @@
         <v>153</v>
       </c>
       <c r="B72" s="2">
-        <v>1000</v>
+        <v>200</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1587,7 +1604,7 @@
         <v>154</v>
       </c>
       <c r="B73" s="2">
-        <v>300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1611,7 +1628,8 @@
         <v>157</v>
       </c>
       <c r="B76" s="2">
-        <v>20</v>
+        <f>INT(Main_Loop_Parameters!B4/Main_Loop_Parameters!B7)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1619,7 +1637,7 @@
         <v>158</v>
       </c>
       <c r="B77" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1635,7 +1653,7 @@
         <v>160</v>
       </c>
       <c r="B79" s="2">
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1643,7 +1661,7 @@
         <v>161</v>
       </c>
       <c r="B80" s="2">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1651,7 +1669,7 @@
         <v>162</v>
       </c>
       <c r="B81" s="2">
-        <v>200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1683,7 +1701,7 @@
         <v>166</v>
       </c>
       <c r="B85" s="2">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1699,7 +1717,7 @@
         <v>168</v>
       </c>
       <c r="B87" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1715,7 +1733,7 @@
         <v>170</v>
       </c>
       <c r="B89" s="2">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1785,7 +1803,7 @@
         <v>178</v>
       </c>
       <c r="B98" s="2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1828,10 +1846,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1859,7 +1877,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="3">
-        <v>200</v>
+        <v>600</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1867,7 +1885,7 @@
         <v>40</v>
       </c>
       <c r="B4" s="3">
-        <v>10000</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1875,7 +1893,7 @@
         <v>41</v>
       </c>
       <c r="B5" s="3">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1883,7 +1901,7 @@
         <v>42</v>
       </c>
       <c r="B6" s="3">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1892,7 +1910,7 @@
       </c>
       <c r="B7" s="3">
         <f>B5+B6</f>
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1960,7 +1978,7 @@
         <v>52</v>
       </c>
       <c r="B16" s="3">
-        <v>1000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2052,7 +2070,7 @@
         <v>64</v>
       </c>
       <c r="B28" s="3">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2060,7 +2078,7 @@
         <v>65</v>
       </c>
       <c r="B29" s="3">
-        <v>1.05</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2068,7 +2086,7 @@
         <v>66</v>
       </c>
       <c r="B30" s="3">
-        <v>1.004</v>
+        <v>1.002</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2076,7 +2094,7 @@
         <v>67</v>
       </c>
       <c r="B31" s="3">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2087,7 +2105,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -2095,45 +2113,45 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>70</v>
       </c>
       <c r="B34" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>71</v>
       </c>
       <c r="B35" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>72</v>
       </c>
       <c r="B36" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>73</v>
       </c>
       <c r="B37" s="3">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>74</v>
       </c>
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -2141,7 +2159,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -2149,7 +2167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>77</v>
       </c>
@@ -2157,7 +2175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>78</v>
       </c>
@@ -2165,7 +2183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -2173,7 +2191,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>80</v>
       </c>
@@ -2181,7 +2199,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>81</v>
       </c>
@@ -2189,13 +2207,16 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>82</v>
       </c>
       <c r="B46" s="3"/>
-    </row>
-    <row r="47" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E46" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>83</v>
       </c>
@@ -2203,7 +2224,7 @@
         <v>-1E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>84</v>
       </c>
@@ -2223,7 +2244,7 @@
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -2384,7 +2405,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2437,7 +2458,8 @@
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <v>0.08</v>
+        <f>1/12</f>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D2" s="3">
         <v>0.1</v>
@@ -2449,7 +2471,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="1">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H2" s="2">
         <v>0.1</v>
@@ -2466,19 +2488,20 @@
         <v>1</v>
       </c>
       <c r="C3" s="2">
-        <v>0.08</v>
+        <f t="shared" ref="C3:C13" si="0">1/12</f>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D3" s="3">
         <v>0.01</v>
       </c>
       <c r="E3" s="1">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
       </c>
       <c r="G3" s="1">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H3" s="2">
         <v>0.1</v>
@@ -2495,22 +2518,23 @@
         <v>2</v>
       </c>
       <c r="C4" s="2">
-        <v>0.08</v>
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D4" s="3">
         <v>0.01</v>
       </c>
       <c r="E4" s="1">
+        <v>100</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
         <v>50</v>
       </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1">
-        <v>20</v>
-      </c>
       <c r="H4" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I4" s="1">
         <v>48000</v>
@@ -2524,22 +2548,23 @@
         <v>3</v>
       </c>
       <c r="C5" s="2">
-        <v>0.08</v>
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D5" s="3">
         <v>0.01</v>
       </c>
       <c r="E5" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
       <c r="G5" s="1">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="H5" s="2">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="I5" s="1">
         <v>303000</v>
@@ -2553,22 +2578,23 @@
         <v>4</v>
       </c>
       <c r="C6" s="2">
-        <v>0.08</v>
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D6" s="3">
         <v>0.01</v>
       </c>
       <c r="E6" s="1">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
       </c>
       <c r="G6" s="1">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="H6" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I6" s="1">
         <v>56000</v>
@@ -2582,22 +2608,23 @@
         <v>5</v>
       </c>
       <c r="C7" s="2">
-        <v>0.08</v>
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D7" s="3">
         <v>0.01</v>
       </c>
       <c r="E7" s="1">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
       </c>
       <c r="G7" s="1">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H7" s="2">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="I7" s="1">
         <v>18000</v>
@@ -2611,13 +2638,14 @@
         <v>6</v>
       </c>
       <c r="C8" s="2">
-        <v>0.08</v>
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D8" s="3">
         <v>0.01</v>
       </c>
       <c r="E8" s="1">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
@@ -2626,7 +2654,7 @@
         <v>50</v>
       </c>
       <c r="H8" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I8" s="1">
         <v>111000</v>
@@ -2640,22 +2668,23 @@
         <v>7</v>
       </c>
       <c r="C9" s="2">
-        <v>0.08</v>
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D9" s="3">
         <v>0.01</v>
       </c>
       <c r="E9" s="1">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
       <c r="G9" s="1">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H9" s="2">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="I9" s="1">
         <v>19000</v>
@@ -2669,19 +2698,20 @@
         <v>8</v>
       </c>
       <c r="C10" s="2">
-        <v>0.08</v>
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D10" s="3">
         <v>0.01</v>
       </c>
       <c r="E10" s="1">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
       </c>
       <c r="G10" s="1">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="H10" s="2">
         <v>0.1</v>
@@ -2698,22 +2728,23 @@
         <v>9</v>
       </c>
       <c r="C11" s="2">
-        <v>0.08</v>
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D11" s="3">
         <v>0.01</v>
       </c>
       <c r="E11" s="1">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
       </c>
       <c r="G11" s="1">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="H11" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I11" s="1">
         <v>23000</v>
@@ -2727,19 +2758,20 @@
         <v>10</v>
       </c>
       <c r="C12" s="2">
-        <v>0.08</v>
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D12" s="3">
         <v>0.01</v>
       </c>
       <c r="E12" s="1">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
       </c>
       <c r="G12" s="1">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H12" s="2">
         <v>0.1</v>
@@ -2756,19 +2788,20 @@
         <v>11</v>
       </c>
       <c r="C13" s="2">
-        <v>0.08</v>
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D13" s="3">
         <v>0.01</v>
       </c>
       <c r="E13" s="1">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
       </c>
       <c r="G13" s="1">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="H13" s="2">
         <v>0.1</v>

</xml_diff>

<commit_message>
testing to fix capital demand
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayman/Desktop/FYP_project/Vulcan/InitializationData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D87F3ED-6411-1740-ADDF-3830811DF9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4408419A-C505-0342-9350-E441C46A8BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1020,14 +1020,14 @@
   </sheetPr>
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="115" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="115" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1309,7 +1309,7 @@
         <v>118</v>
       </c>
       <c r="B36" s="16">
-        <v>10000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1848,7 +1848,7 @@
   </sheetPr>
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="150" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1877,7 +1877,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="3">
-        <v>600</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
test check sales for production
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayman/Desktop/FYP_project/Vulcan/InitializationData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4408419A-C505-0342-9350-E441C46A8BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F1993E-C0FB-3C40-9706-56ABEBA402DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initialization_Parameters" sheetId="1" r:id="rId1"/>
@@ -1020,8 +1020,8 @@
   </sheetPr>
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="115" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A36" zoomScale="115" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="B46" s="2">
         <f>INT(Main_Loop_Parameters!B4/Main_Loop_Parameters!B7)</f>
-        <v>4</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1629,7 +1629,7 @@
       </c>
       <c r="B76" s="2">
         <f>INT(Main_Loop_Parameters!B4/Main_Loop_Parameters!B7)</f>
-        <v>4</v>
+        <v>41</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1848,8 +1848,8 @@
   </sheetPr>
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1885,7 +1885,7 @@
         <v>40</v>
       </c>
       <c r="B4" s="3">
-        <v>200</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1978,7 +1978,7 @@
         <v>52</v>
       </c>
       <c r="B16" s="3">
-        <v>10</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2404,8 +2404,8 @@
   </sheetPr>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Loop simulations with random params each time
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayman/Desktop/FYP_project/Vulcan/InitializationData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4408419A-C505-0342-9350-E441C46A8BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE691D95-4A18-CF44-ABF3-BA1EA14594AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initialization_Parameters" sheetId="1" r:id="rId1"/>
@@ -1020,8 +1020,8 @@
   </sheetPr>
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="115" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="B46" s="2">
         <f>INT(Main_Loop_Parameters!B4/Main_Loop_Parameters!B7)</f>
-        <v>4</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1629,7 +1629,7 @@
       </c>
       <c r="B76" s="2">
         <f>INT(Main_Loop_Parameters!B4/Main_Loop_Parameters!B7)</f>
-        <v>4</v>
+        <v>41</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1848,8 +1848,8 @@
   </sheetPr>
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1885,7 +1885,7 @@
         <v>40</v>
       </c>
       <c r="B4" s="3">
-        <v>200</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1978,7 +1978,7 @@
         <v>52</v>
       </c>
       <c r="B16" s="3">
-        <v>10</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2405,7 +2405,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Implementation of Bayesian Parameter Estimation
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayman/Desktop/FYP_project/Vulcan/InitializationData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE691D95-4A18-CF44-ABF3-BA1EA14594AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE1FF68-9788-AF4B-8475-4D7C243EC860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1849,7 +1849,7 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1877,7 +1877,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="3">
-        <v>200</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Auto param estimation works now
</commit_message>
<xml_diff>
--- a/InitializationData/Simulation_Parameters.xlsx
+++ b/InitializationData/Simulation_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayman/Desktop/FYP_project/Vulcan/InitializationData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE1FF68-9788-AF4B-8475-4D7C243EC860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00FE4DD-ABB2-C34E-8A1C-2F43C4B6935B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initialization_Parameters" sheetId="1" r:id="rId1"/>
@@ -610,7 +610,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -631,8 +631,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -642,6 +648,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -665,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -711,6 +723,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1020,8 +1044,8 @@
   </sheetPr>
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+    <sheetView topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1062,7 +1086,7 @@
       <c r="A5" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="17">
         <v>0.5</v>
       </c>
     </row>
@@ -1095,7 +1119,7 @@
         <v>92</v>
       </c>
       <c r="B9" s="2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1126,7 +1150,7 @@
       <c r="A13" t="s">
         <v>96</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="17">
         <v>0.2</v>
       </c>
     </row>
@@ -1191,7 +1215,7 @@
         <v>104</v>
       </c>
       <c r="B21" s="16">
-        <v>500</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1222,8 +1246,8 @@
       <c r="A25" t="s">
         <v>108</v>
       </c>
-      <c r="B25" s="2">
-        <v>4</v>
+      <c r="B25" s="17">
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1279,7 +1303,7 @@
         <v>115</v>
       </c>
       <c r="B32" s="2">
-        <v>999999</v>
+        <v>500</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1294,7 +1318,7 @@
       <c r="A34" t="s">
         <v>117</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="17">
         <v>500</v>
       </c>
     </row>
@@ -1357,7 +1381,7 @@
         <v>124</v>
       </c>
       <c r="B42" s="2">
-        <v>200</v>
+        <v>600</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1365,7 +1389,7 @@
         <v>125</v>
       </c>
       <c r="B43" s="2">
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1390,7 +1414,7 @@
       </c>
       <c r="B46" s="2">
         <f>INT(Main_Loop_Parameters!B4/Main_Loop_Parameters!B7)</f>
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1422,7 +1446,7 @@
         <v>132</v>
       </c>
       <c r="B50" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1430,7 +1454,7 @@
         <v>133</v>
       </c>
       <c r="B51" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1596,7 +1620,7 @@
         <v>153</v>
       </c>
       <c r="B72" s="2">
-        <v>200</v>
+        <v>600</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1629,7 +1653,7 @@
       </c>
       <c r="B76" s="2">
         <f>INT(Main_Loop_Parameters!B4/Main_Loop_Parameters!B7)</f>
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1725,7 +1749,7 @@
         <v>169</v>
       </c>
       <c r="B88" s="2">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1838,6 +1862,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1848,8 +1873,8 @@
   </sheetPr>
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1884,24 +1909,24 @@
       <c r="A4" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="3">
-        <v>2000</v>
+      <c r="B4" s="19">
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="3">
-        <v>36</v>
+      <c r="B5" s="19">
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="3">
-        <v>12</v>
+      <c r="B6" s="19">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1910,7 +1935,7 @@
       </c>
       <c r="B7" s="3">
         <f>B5+B6</f>
-        <v>48</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1939,7 +1964,7 @@
       <c r="A11" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="18">
         <v>2</v>
       </c>
     </row>
@@ -2001,8 +2026,8 @@
       <c r="A19" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="3">
-        <v>1</v>
+      <c r="B19" s="19">
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2234,6 +2259,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2244,8 +2270,8 @@
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2297,14 +2323,16 @@
         <v>27</v>
       </c>
       <c r="B6" s="9">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="9"/>
+      <c r="B7" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
@@ -2326,7 +2354,7 @@
       <c r="A10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="20">
         <v>0.1</v>
       </c>
     </row>
@@ -2334,16 +2362,16 @@
       <c r="A11" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="9">
-        <v>0.2</v>
+      <c r="B11" s="20">
+        <v>0.1</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>184</v>
       </c>
-      <c r="B12" s="3">
-        <v>0.25</v>
+      <c r="B12" s="20">
+        <v>0.2</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2372,7 +2400,7 @@
       <c r="A16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="20">
         <v>0.1</v>
       </c>
     </row>
@@ -2381,19 +2409,20 @@
         <v>36</v>
       </c>
       <c r="B17" s="9">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>185</v>
       </c>
-      <c r="B18" s="3">
-        <v>0.25</v>
+      <c r="B18" s="19">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2405,7 +2434,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2462,7 +2491,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D2" s="3">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E2" s="1">
         <v>100</v>

</xml_diff>